<commit_message>
Implemented Database for task tables, Implemented Add task,
Implemented Database for task tables
   1. Created Task, TaskStage, and
   TaskEmployee tables
Implemented Add task functionality
   1. Users can now add tasks depending
   on their role and associations
Updated Sprint backlog
</commit_message>
<xml_diff>
--- a/Sprints/Sprint3/G4CapstoneProject_Sprint3_Backlog_Burndown.xlsx
+++ b/Sprints/Sprint3/G4CapstoneProject_Sprint3_Backlog_Burndown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmad\Documents\GitHub\Capstone-Project\Sprints\Sprint3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6653EF42-F82E-4189-BD92-F9C9FF65689C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFB30B10-817F-4809-A868-8ED6F54E3F6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5265" yWindow="3990" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -486,7 +486,7 @@
                   <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1531,7 +1531,7 @@
   <dimension ref="A1:F55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1680,7 +1680,7 @@
         <v>1</v>
       </c>
       <c r="E9" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9" s="13" t="s">
         <v>16</v>
@@ -1714,7 +1714,7 @@
         <v>1</v>
       </c>
       <c r="E11" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F11" s="13" t="s">
         <v>16</v>
@@ -1921,7 +1921,7 @@
       </c>
       <c r="E22" s="4">
         <f>SUM(E4:E21)</f>
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F22" s="18"/>
     </row>

</xml_diff>

<commit_message>
Added fixes and more functionality
Added functionality to restrict functionality if not in assigned group

Fixed bug where available employees in create task was not listing.

Made the view wrap each task around in a border

Updated Sprint backlog
</commit_message>
<xml_diff>
--- a/Sprints/Sprint3/G4CapstoneProject_Sprint3_Backlog_Burndown.xlsx
+++ b/Sprints/Sprint3/G4CapstoneProject_Sprint3_Backlog_Burndown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmad\Documents\GitHub\Capstone-Project\Sprints\Sprint3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FCC927C-A395-4199-8BAD-6FD8F2D46F3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9F1E9C5-9A54-45F5-89FA-C09610E7DD28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5265" yWindow="3990" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -486,7 +486,7 @@
                   <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1531,7 +1531,7 @@
   <dimension ref="A1:F55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1776,7 +1776,7 @@
         <v>1</v>
       </c>
       <c r="E14" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F14" s="13" t="s">
         <v>16</v>
@@ -1794,7 +1794,7 @@
         <v>0.5</v>
       </c>
       <c r="E15" s="8">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F15" s="13" t="s">
         <v>16</v>
@@ -1925,7 +1925,7 @@
       </c>
       <c r="E22" s="4">
         <f>SUM(E4:E21)</f>
-        <v>8</v>
+        <v>6.5</v>
       </c>
       <c r="F22" s="18"/>
     </row>

</xml_diff>